<commit_message>
Vse podatke zdruzil v skupno tabelo. Odstranil kodo, ki je ne rabim
</commit_message>
<xml_diff>
--- a/podatki/izobrazba-po-regijah.xlsx
+++ b/podatki/izobrazba-po-regijah.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tjazerzen/Documents/fakulteta/letnik2/letnik2 - predmeti/APPR/projekt/analiza_bolniskega_staleza/podatki/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B14BCC-C6A5-1E48-A87C-4B6CCA0CB7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB8240D-56AB-C948-99A9-46C7B2EBBB14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -212,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="37">
   <si>
     <t>Izobrazba - SKUPAJ</t>
   </si>
@@ -274,9 +274,6 @@
     <t>Posavska</t>
   </si>
   <si>
-    <t>Jugovzhodna Slovenija</t>
-  </si>
-  <si>
     <t>Osrednjeslovenska</t>
   </si>
   <si>
@@ -323,6 +320,9 @@
   </si>
   <si>
     <t>Spol</t>
+  </si>
+  <si>
+    <t>Jugovzhodna</t>
   </si>
 </sst>
 </file>
@@ -692,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N140"/>
+  <dimension ref="A1:N139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="140" workbookViewId="0">
+      <selection activeCell="A134" sqref="A134:XFD134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -719,13 +719,13 @@
     </row>
     <row r="3" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
@@ -1074,7 +1074,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>13</v>
@@ -1118,7 +1118,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>13</v>
@@ -1162,7 +1162,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>13</v>
@@ -1206,7 +1206,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>13</v>
@@ -1250,7 +1250,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>13</v>
@@ -1294,7 +1294,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>13</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>12</v>
@@ -1379,7 +1379,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>14</v>
@@ -1423,7 +1423,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>15</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>16</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>17</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>18</v>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>19</v>
@@ -1643,10 +1643,10 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>13</v>
@@ -1687,10 +1687,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>13</v>
@@ -1731,10 +1731,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>13</v>
@@ -1775,10 +1775,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>13</v>
@@ -1819,10 +1819,10 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>13</v>
@@ -1863,10 +1863,10 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>13</v>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>12</v>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>14</v>
@@ -1995,7 +1995,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>15</v>
@@ -2039,7 +2039,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>16</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>17</v>
@@ -2127,7 +2127,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>18</v>
@@ -2171,7 +2171,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>19</v>
@@ -2215,10 +2215,10 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>13</v>
@@ -2259,10 +2259,10 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>13</v>
@@ -2303,10 +2303,10 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>13</v>
@@ -2347,10 +2347,10 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>13</v>
@@ -2391,10 +2391,10 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>13</v>
@@ -2435,10 +2435,10 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>13</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>12</v>
@@ -2523,7 +2523,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>14</v>
@@ -2567,7 +2567,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>15</v>
@@ -2611,7 +2611,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>16</v>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>17</v>
@@ -2699,7 +2699,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>18</v>
@@ -2743,7 +2743,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>19</v>
@@ -2787,10 +2787,10 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>13</v>
@@ -2831,10 +2831,10 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>13</v>
@@ -2875,10 +2875,10 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>13</v>
@@ -2919,10 +2919,10 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>13</v>
@@ -2963,10 +2963,10 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>13</v>
@@ -3007,10 +3007,10 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>13</v>
@@ -3051,7 +3051,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>12</v>
@@ -3095,7 +3095,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>14</v>
@@ -3139,7 +3139,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>15</v>
@@ -3183,7 +3183,7 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>16</v>
@@ -3227,7 +3227,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>17</v>
@@ -3271,7 +3271,7 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>18</v>
@@ -3315,7 +3315,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>19</v>
@@ -3359,10 +3359,10 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>13</v>
@@ -3403,10 +3403,10 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>13</v>
@@ -3447,10 +3447,10 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>13</v>
@@ -3491,10 +3491,10 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>13</v>
@@ -3535,10 +3535,10 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>13</v>
@@ -3579,10 +3579,10 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>13</v>
@@ -3623,7 +3623,7 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>12</v>
@@ -3667,7 +3667,7 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>14</v>
@@ -3711,7 +3711,7 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>15</v>
@@ -3755,7 +3755,7 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>16</v>
@@ -3799,7 +3799,7 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>17</v>
@@ -3843,7 +3843,7 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>18</v>
@@ -3887,7 +3887,7 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>19</v>
@@ -3931,10 +3931,10 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>13</v>
@@ -3975,10 +3975,10 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>13</v>
@@ -4019,10 +4019,10 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>13</v>
@@ -4063,10 +4063,10 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>13</v>
@@ -4107,10 +4107,10 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>13</v>
@@ -4151,10 +4151,10 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>13</v>
@@ -4195,7 +4195,7 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>12</v>
@@ -4239,7 +4239,7 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>14</v>
@@ -4283,7 +4283,7 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>15</v>
@@ -4327,7 +4327,7 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>16</v>
@@ -4371,7 +4371,7 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>17</v>
@@ -4415,7 +4415,7 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>18</v>
@@ -4459,7 +4459,7 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>19</v>
@@ -4503,10 +4503,10 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>13</v>
@@ -4547,10 +4547,10 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>13</v>
@@ -4591,10 +4591,10 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>13</v>
@@ -4635,10 +4635,10 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>13</v>
@@ -4679,10 +4679,10 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>13</v>
@@ -4723,10 +4723,10 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>13</v>
@@ -4767,7 +4767,7 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>12</v>
@@ -4811,7 +4811,7 @@
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>14</v>
@@ -4855,7 +4855,7 @@
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>15</v>
@@ -4899,7 +4899,7 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>16</v>
@@ -4943,7 +4943,7 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>17</v>
@@ -4987,7 +4987,7 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>18</v>
@@ -5031,7 +5031,7 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>19</v>
@@ -5075,10 +5075,10 @@
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>13</v>
@@ -5119,10 +5119,10 @@
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>13</v>
@@ -5163,10 +5163,10 @@
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>13</v>
@@ -5207,10 +5207,10 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>13</v>
@@ -5251,10 +5251,10 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>13</v>
@@ -5295,10 +5295,10 @@
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>13</v>
@@ -5650,7 +5650,7 @@
         <v>2019</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>13</v>
@@ -5694,7 +5694,7 @@
         <v>2019</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>13</v>
@@ -5738,7 +5738,7 @@
         <v>2019</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>13</v>
@@ -5782,7 +5782,7 @@
         <v>2019</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>13</v>
@@ -5826,7 +5826,7 @@
         <v>2019</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>13</v>
@@ -5870,7 +5870,7 @@
         <v>2019</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>13</v>
@@ -5911,7 +5911,7 @@
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>12</v>
@@ -5955,7 +5955,7 @@
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>14</v>
@@ -5999,7 +5999,7 @@
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>15</v>
@@ -6043,7 +6043,7 @@
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>16</v>
@@ -6087,7 +6087,7 @@
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>17</v>
@@ -6131,7 +6131,7 @@
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>18</v>
@@ -6175,7 +6175,7 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>19</v>
@@ -6219,10 +6219,10 @@
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>13</v>
@@ -6263,10 +6263,10 @@
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>13</v>
@@ -6307,10 +6307,10 @@
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>13</v>
@@ -6351,10 +6351,10 @@
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>13</v>
@@ -6395,10 +6395,10 @@
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>13</v>
@@ -6439,10 +6439,10 @@
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>13</v>
@@ -6482,15 +6482,10 @@
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A134" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A135" s="4"/>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A140" s="4"/>
+      <c r="A134" s="4"/>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A139" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>